<commit_message>
Cam capture and temp dir ops complete
</commit_message>
<xml_diff>
--- a/Database_format.xlsx
+++ b/Database_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Git stuff\Safe-Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8FDE27-8195-4542-9187-DC4CEC7899C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6C2BC2-99D3-4A49-B120-9468FC9322C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,39 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Encrypted_files</t>
   </si>
   <si>
-    <t>pid</t>
-  </si>
-  <si>
-    <t>date_updated</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>private_key(plaintext)</t>
   </si>
   <si>
-    <t>profile_pic</t>
-  </si>
-  <si>
     <t>four_digit_pass(hashed)</t>
   </si>
   <si>
     <t>owner (foreigh key user)</t>
   </si>
   <si>
-    <t>auth_image</t>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>profile_pic_filename</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>date_uploaded</t>
   </si>
 </sst>
 </file>
@@ -488,101 +485,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:K8"/>
+  <dimension ref="A3:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22.21875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="20.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.21875" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="10" max="11" width="19.21875" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="I5" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="9"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>